<commit_message>
Changes for version 1.5.5
</commit_message>
<xml_diff>
--- a/provider.model.standard.excel/src/main/resources/defaultInputData/MOGLiCC_JavaBeanModel_Testdaten.xlsx
+++ b/provider.model.standard.excel/src/main/resources/defaultInputData/MOGLiCC_JavaBeanModel_Testdaten.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="93">
   <si>
     <t>First cell</t>
   </si>
@@ -68,9 +68,6 @@
     <t>Person4</t>
   </si>
   <si>
-    <t>address</t>
-  </si>
-  <si>
     <t>country</t>
   </si>
   <si>
@@ -83,9 +80,6 @@
     <t>Street</t>
   </si>
   <si>
-    <t>streetNumber</t>
-  </si>
-  <si>
     <t>DE</t>
   </si>
   <si>
@@ -104,15 +98,9 @@
     <t>Denver</t>
   </si>
   <si>
-    <t>Hafenstr.</t>
-  </si>
-  <si>
     <t>5th Avenue</t>
   </si>
   <si>
-    <t>Köpmangatan</t>
-  </si>
-  <si>
     <t>Address2</t>
   </si>
   <si>
@@ -155,13 +143,7 @@
     <t>Düsseldorf</t>
   </si>
   <si>
-    <t>Königsallee</t>
-  </si>
-  <si>
     <t>Freiburg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Wentzingerstraße </t>
   </si>
   <si>
     <t>* Note, that attribute names must match exactly the ones of the model file of the StandardModelProvider. If not matching, the excel data do not enrich existing attributes of the standard model but add new attributes!</t>
@@ -201,12 +183,150 @@
       <t>*</t>
     </r>
   </si>
+  <si>
+    <t>Address1, Address3</t>
+  </si>
+  <si>
+    <t>addresses</t>
+  </si>
+  <si>
+    <t>Contact1</t>
+  </si>
+  <si>
+    <t>Contact2</t>
+  </si>
+  <si>
+    <t>Contact4</t>
+  </si>
+  <si>
+    <t>Contact3</t>
+  </si>
+  <si>
+    <t>mobile</t>
+  </si>
+  <si>
+    <t>0151/100234</t>
+  </si>
+  <si>
+    <t>0178/443367</t>
+  </si>
+  <si>
+    <t>0182/464748</t>
+  </si>
+  <si>
+    <t>0182/929392</t>
+  </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>tim.mueller@gmx.de</t>
+  </si>
+  <si>
+    <t>gustavsons@itsm.com</t>
+  </si>
+  <si>
+    <t>maggys@uni.se</t>
+  </si>
+  <si>
+    <t>alice.wonder@nasa.com</t>
+  </si>
+  <si>
+    <t>Office1</t>
+  </si>
+  <si>
+    <t>Office2</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>HeadQuarter</t>
+  </si>
+  <si>
+    <t>outpost</t>
+  </si>
+  <si>
+    <t>type</t>
+  </si>
+  <si>
+    <t>HEAD</t>
+  </si>
+  <si>
+    <t>BRANCH</t>
+  </si>
+  <si>
+    <t>address</t>
+  </si>
+  <si>
+    <t>AddressOffice1</t>
+  </si>
+  <si>
+    <t>AddressOffice2</t>
+  </si>
+  <si>
+    <t>members</t>
+  </si>
+  <si>
+    <t>Member1, Member2, Member4, Member5</t>
+  </si>
+  <si>
+    <t>Member2, Member4</t>
+  </si>
+  <si>
+    <t>active</t>
+  </si>
+  <si>
+    <t>true</t>
+  </si>
+  <si>
+    <t>false</t>
+  </si>
+  <si>
+    <t>role</t>
+  </si>
+  <si>
+    <t>CHIEF</t>
+  </si>
+  <si>
+    <t>GUEST</t>
+  </si>
+  <si>
+    <t>STANDARD</t>
+  </si>
+  <si>
+    <t>offices</t>
+  </si>
+  <si>
+    <t>Office1, Office2</t>
+  </si>
+  <si>
+    <t>Hafenstr. 12</t>
+  </si>
+  <si>
+    <t>Köpmangatan 5</t>
+  </si>
+  <si>
+    <t>Wenzingerstraße  24</t>
+  </si>
+  <si>
+    <t>Köpmangatan 4</t>
+  </si>
+  <si>
+    <t>Königsallee 101a</t>
+  </si>
+  <si>
+    <t>person</t>
+  </si>
+  <si>
+    <t>contact</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -226,6 +346,14 @@
       <b/>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -364,10 +492,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -394,8 +523,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -702,23 +835,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:S26"/>
+  <dimension ref="B2:T35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="19.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.140625" customWidth="1"/>
+    <col min="6" max="6" width="23" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.140625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="14.5703125" customWidth="1"/>
     <col min="19" max="19" width="11.42578125" style="25"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="3" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B3" s="17" t="s">
         <v>0</v>
       </c>
@@ -731,12 +865,17 @@
       <c r="E3" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="F3" s="19" t="s">
-        <v>17</v>
-      </c>
-      <c r="G3" s="2"/>
-    </row>
-    <row r="4" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="F3" s="18" t="s">
+        <v>92</v>
+      </c>
+      <c r="G3" s="19" t="s">
+        <v>48</v>
+      </c>
+      <c r="H3" s="2"/>
+      <c r="S3"/>
+      <c r="T3" s="25"/>
+    </row>
+    <row r="4" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B4" s="20" t="s">
         <v>13</v>
       </c>
@@ -749,11 +888,16 @@
       <c r="E4" s="14">
         <v>25</v>
       </c>
-      <c r="F4" s="10" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="F4" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="G4" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="S4"/>
+      <c r="T4" s="25"/>
+    </row>
+    <row r="5" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B5" s="20" t="s">
         <v>14</v>
       </c>
@@ -766,11 +910,16 @@
       <c r="E5" s="14">
         <v>71</v>
       </c>
-      <c r="F5" s="21" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="F5" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="G5" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="S5"/>
+      <c r="T5" s="25"/>
+    </row>
+    <row r="6" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B6" s="20" t="s">
         <v>15</v>
       </c>
@@ -783,9 +932,14 @@
       <c r="E6" s="14">
         <v>44</v>
       </c>
-      <c r="F6" s="10"/>
-    </row>
-    <row r="7" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F6" s="14" t="s">
+        <v>52</v>
+      </c>
+      <c r="G6" s="10"/>
+      <c r="S6"/>
+      <c r="T6" s="25"/>
+    </row>
+    <row r="7" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B7" s="22" t="s">
         <v>16</v>
       </c>
@@ -798,230 +952,457 @@
       <c r="E7" s="16">
         <v>9</v>
       </c>
-      <c r="F7" s="12" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="8" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="F7" s="16" t="s">
+        <v>51</v>
+      </c>
+      <c r="G7" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="S7"/>
+      <c r="T7" s="25"/>
+    </row>
+    <row r="8" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B8" s="1"/>
     </row>
-    <row r="12" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B12" s="5" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B13" s="1" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="14" spans="2:7" x14ac:dyDescent="0.25">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="14" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B14" s="2" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="15" spans="2:7" x14ac:dyDescent="0.25">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="15" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B15" s="6" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="16" spans="2:7" x14ac:dyDescent="0.25">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="16" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B16" s="4" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="17" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B17" s="3" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="18" spans="2:8" x14ac:dyDescent="0.25">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="18" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B18" s="24" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="20" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="21" spans="2:8" x14ac:dyDescent="0.25">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="20" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G20" s="14"/>
+      <c r="H20" s="14"/>
+      <c r="I20" s="14"/>
+    </row>
+    <row r="21" spans="2:9" x14ac:dyDescent="0.25">
       <c r="C21" s="7"/>
       <c r="D21" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="E21" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="E21" s="13" t="s">
+      <c r="F21" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="F21" s="13" t="s">
+      <c r="G21" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="G21" s="13" t="s">
+      <c r="H21" s="14"/>
+      <c r="I21" s="14"/>
+    </row>
+    <row r="22" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="C22" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="D22" s="14" t="s">
         <v>21</v>
-      </c>
-      <c r="H21" s="8" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="22" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="C22" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="D22" s="14" t="s">
-        <v>23</v>
       </c>
       <c r="E22" s="14">
         <v>20359</v>
       </c>
       <c r="F22" s="14" t="s">
-        <v>26</v>
-      </c>
-      <c r="G22" s="14" t="s">
-        <v>29</v>
-      </c>
-      <c r="H22" s="10">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="23" spans="2:8" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+      <c r="G22" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="H22" s="14"/>
+      <c r="I22" s="14"/>
+    </row>
+    <row r="23" spans="2:9" x14ac:dyDescent="0.25">
       <c r="C23" s="15" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="D23" s="14" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="E23" s="14">
         <v>11131</v>
       </c>
       <c r="F23" s="14" t="s">
-        <v>27</v>
-      </c>
-      <c r="G23" s="14" t="s">
-        <v>31</v>
-      </c>
-      <c r="H23" s="10">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="24" spans="2:8" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+      <c r="G23" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="H23" s="14"/>
+      <c r="I23" s="14"/>
+    </row>
+    <row r="24" spans="2:9" x14ac:dyDescent="0.25">
       <c r="C24" s="9" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="D24" s="14" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E24" s="14">
         <v>40215</v>
       </c>
       <c r="F24" s="23" t="s">
-        <v>45</v>
-      </c>
-      <c r="G24" s="23" t="s">
-        <v>46</v>
-      </c>
-      <c r="H24" s="10">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="25" spans="2:8" x14ac:dyDescent="0.25">
+        <v>41</v>
+      </c>
+      <c r="G24" s="26" t="s">
+        <v>90</v>
+      </c>
+      <c r="H24" s="14"/>
+      <c r="I24" s="14"/>
+    </row>
+    <row r="25" spans="2:9" x14ac:dyDescent="0.25">
       <c r="C25" s="9" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="D25" s="14" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E25" s="23">
         <v>79106</v>
       </c>
       <c r="F25" s="23" t="s">
-        <v>47</v>
-      </c>
-      <c r="G25" s="23" t="s">
-        <v>48</v>
-      </c>
-      <c r="H25" s="10">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="26" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C26" s="11" t="s">
-        <v>44</v>
-      </c>
-      <c r="D26" s="16" t="s">
+        <v>42</v>
+      </c>
+      <c r="G25" s="26" t="s">
+        <v>88</v>
+      </c>
+      <c r="H25" s="14"/>
+      <c r="I25" s="14"/>
+    </row>
+    <row r="26" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="C26" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="D26" s="23" t="s">
+        <v>22</v>
+      </c>
+      <c r="E26" s="14">
+        <v>11131</v>
+      </c>
+      <c r="F26" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="E26" s="16">
+      <c r="G26" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="H26" s="14"/>
+      <c r="I26" s="14"/>
+    </row>
+    <row r="27" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="C27" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="D27" s="23" t="s">
+        <v>23</v>
+      </c>
+      <c r="E27" s="14">
         <v>80204</v>
       </c>
-      <c r="F26" s="16" t="s">
-        <v>28</v>
-      </c>
-      <c r="G26" s="16" t="s">
-        <v>30</v>
-      </c>
-      <c r="H26" s="12">
-        <v>392</v>
+      <c r="F27" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="G27" s="26"/>
+      <c r="H27" s="14"/>
+      <c r="I27" s="14"/>
+    </row>
+    <row r="28" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C28" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="D28" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="E28" s="16">
+        <v>80204</v>
+      </c>
+      <c r="F28" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="G28" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="H28" s="14"/>
+      <c r="I28" s="14"/>
+    </row>
+    <row r="29" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="G29" s="14"/>
+      <c r="H29" s="14"/>
+      <c r="I29" s="14"/>
+    </row>
+    <row r="30" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="31" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="C31" s="7"/>
+      <c r="D31" s="13" t="s">
+        <v>91</v>
+      </c>
+      <c r="E31" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="F31" s="8" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="32" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="C32" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="D32" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="E32" s="14" t="s">
+        <v>54</v>
+      </c>
+      <c r="F32" s="27" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="33" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C33" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="D33" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="E33" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="F33" s="27" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="34" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C34" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="D34" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="E34" s="14" t="s">
+        <v>56</v>
+      </c>
+      <c r="F34" s="27" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="35" spans="3:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C35" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="D35" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="E35" s="16" t="s">
+        <v>57</v>
+      </c>
+      <c r="F35" s="28" t="s">
+        <v>62</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="F32" r:id="rId1"/>
+    <hyperlink ref="F33" r:id="rId2"/>
+    <hyperlink ref="F34" r:id="rId3"/>
+    <hyperlink ref="F35" r:id="rId4"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId5"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C3:D9"/>
+  <dimension ref="B3:G15"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="4" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16" customWidth="1"/>
+    <col min="7" max="7" width="39" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="15.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="4" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="4" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C4" s="7"/>
-      <c r="D4" s="8" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="5" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="D4" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="E4" s="13" t="s">
+        <v>77</v>
+      </c>
+      <c r="F4" s="13" t="s">
+        <v>80</v>
+      </c>
+      <c r="G4" s="8" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C5" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="D5" s="14">
+        <v>123</v>
+      </c>
+      <c r="E5" s="14" t="s">
+        <v>78</v>
+      </c>
+      <c r="F5" s="14" t="s">
+        <v>83</v>
+      </c>
+      <c r="G5" s="10" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C6" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="D6" s="14">
+        <v>321</v>
+      </c>
+      <c r="E6" s="14" t="s">
+        <v>78</v>
+      </c>
+      <c r="F6" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="G6" s="10" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C7" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="D7" s="14">
+        <v>22</v>
+      </c>
+      <c r="E7" s="14" t="s">
+        <v>78</v>
+      </c>
+      <c r="F7" s="14" t="s">
+        <v>83</v>
+      </c>
+      <c r="G7" s="10" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="8" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C8" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="D8" s="14">
+        <v>4</v>
+      </c>
+      <c r="E8" s="14" t="s">
+        <v>79</v>
+      </c>
+      <c r="F8" s="14" t="s">
+        <v>82</v>
+      </c>
+      <c r="G8" s="10" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="9" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C9" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="D5" s="10">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="6" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C6" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="D6" s="10">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="7" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C7" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="D7" s="10">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="8" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C8" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="D8" s="10">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="9" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C9" s="11" t="s">
-        <v>39</v>
-      </c>
-      <c r="D9" s="12">
+      <c r="D9" s="16">
         <v>47</v>
+      </c>
+      <c r="E9" s="16" t="s">
+        <v>78</v>
+      </c>
+      <c r="F9" s="16" t="s">
+        <v>83</v>
+      </c>
+      <c r="G9" s="12" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="12" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="13" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B13" s="7"/>
+      <c r="C13" s="13" t="s">
+        <v>65</v>
+      </c>
+      <c r="D13" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="E13" s="13" t="s">
+        <v>71</v>
+      </c>
+      <c r="F13" s="8" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="14" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B14" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="C14" s="14" t="s">
+        <v>66</v>
+      </c>
+      <c r="D14" s="14" t="s">
+        <v>69</v>
+      </c>
+      <c r="E14" s="14" t="s">
+        <v>72</v>
+      </c>
+      <c r="F14" s="10" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="15" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B15" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="C15" s="16" t="s">
+        <v>67</v>
+      </c>
+      <c r="D15" s="16" t="s">
+        <v>70</v>
+      </c>
+      <c r="E15" s="16" t="s">
+        <v>73</v>
+      </c>
+      <c r="F15" s="12" t="s">
+        <v>76</v>
       </c>
     </row>
   </sheetData>

</xml_diff>